<commit_message>
Review of first release of the Product Definition
</commit_message>
<xml_diff>
--- a/PM/Deliverables Tracking.xlsx
+++ b/PM/Deliverables Tracking.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="140000" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
   <si>
     <t>Deliverables Tracking</t>
   </si>
@@ -37,6 +37,21 @@
   </si>
   <si>
     <t>Product Definition.txt</t>
+  </si>
+  <si>
+    <t>Hardware Block Diagram</t>
+  </si>
+  <si>
+    <t>Product Architecture</t>
+  </si>
+  <si>
+    <t>Major Components BOM</t>
+  </si>
+  <si>
+    <t>Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I will order parts on Monday to make sure they are in house by Saturday. If you do not get me the parts order by then you may not be able to build you project. </t>
   </si>
 </sst>
 </file>
@@ -44,7 +59,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
-    <numFmt numFmtId="166" formatCode="m/d/yy;@"/>
+    <numFmt numFmtId="164" formatCode="m/d/yy;@"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -117,7 +132,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="7">
+  <cellStyleXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -125,23 +140,40 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="7">
+  <cellStyles count="15">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -471,7 +503,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B7"/>
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C12" sqref="C12"/>
@@ -479,34 +511,37 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="20.33203125" customWidth="1"/>
+    <col min="1" max="1" width="21.5" customWidth="1"/>
     <col min="2" max="2" width="7.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" ht="17" thickBot="1">
+    <row r="1" spans="1:3" ht="17" thickBot="1">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:2" ht="17" thickBot="1">
+    <row r="2" spans="1:3" ht="17" thickBot="1">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="4" t="s">
+    <row r="4" spans="1:3">
+      <c r="A4" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="3">
+    <row r="5" spans="1:3">
+      <c r="A5" s="4">
         <v>42630</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="6" spans="1:2">
+      <c r="C5" s="3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -514,12 +549,44 @@
         <v>42634</v>
       </c>
     </row>
-    <row r="7" spans="1:2">
+    <row r="7" spans="1:3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
       <c r="B7" s="2">
         <v>42634</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" s="5">
+        <v>42634</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="2">
+        <v>42639</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="2">
+        <v>42639</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2">
+        <v>42639</v>
+      </c>
+      <c r="C12" t="s">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated Deliverables Tracking and Added Presentation slides
</commit_message>
<xml_diff>
--- a/PM/Deliverables Tracking.xlsx
+++ b/PM/Deliverables Tracking.xlsx
@@ -9,7 +9,7 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" iterateDelta="1E-4" concurrentCalc="0"/>
+  <calcPr calcId="140001" calcOnSave="0" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
   <si>
     <t>The Engineer Accelerator September 2016</t>
   </si>
@@ -108,9 +108,6 @@
     <t>Estimate Hours for Full BOM, Manfucaturing Package, and Bring Up</t>
   </si>
   <si>
-    <t>DRC is cleared</t>
-  </si>
-  <si>
     <t>Time</t>
   </si>
   <si>
@@ -120,9 +117,6 @@
     <t>I will order parts on Monday to make sure they are in house by Saturday. If you do not get me the parts order by then you may not be able to build you project.</t>
   </si>
   <si>
-    <t>ERC Cleared</t>
-  </si>
-  <si>
     <t>By end of class</t>
   </si>
   <si>
@@ -130,6 +124,15 @@
   </si>
   <si>
     <t>Choose a method for keeping track of your task list</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matched Guidelines. ERC Cleared. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Matched Guidelines. </t>
+  </si>
+  <si>
+    <t>Matched Guidelines. DRC is cleared</t>
   </si>
 </sst>
 </file>
@@ -859,7 +862,7 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -893,7 +896,7 @@
         <v>3</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D5" t="s">
         <v>4</v>
@@ -976,10 +979,10 @@
         <v>42639</v>
       </c>
       <c r="C14" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="D14" s="5" t="s">
         <v>31</v>
-      </c>
-      <c r="D14" s="5" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30">
@@ -1025,6 +1028,9 @@
       <c r="C18" s="5" t="s">
         <v>19</v>
       </c>
+      <c r="D18" t="s">
+        <v>36</v>
+      </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="5" t="s">
@@ -1037,7 +1043,7 @@
         <v>19</v>
       </c>
       <c r="D19" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1051,7 +1057,7 @@
         <v>19</v>
       </c>
       <c r="D20" t="s">
-        <v>29</v>
+        <v>37</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1078,7 +1084,7 @@
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="3" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B23" s="12">
         <v>42644</v>
@@ -1100,7 +1106,7 @@
         <v>42644</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="30">
@@ -1111,7 +1117,7 @@
         <v>42644</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1122,7 +1128,7 @@
         <v>42648</v>
       </c>
       <c r="C28" s="5" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1133,7 +1139,7 @@
         <v>42644</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:4">

</xml_diff>

<commit_message>
Added portfolios folders to student folders
</commit_message>
<xml_diff>
--- a/PM/Deliverables Tracking.xlsx
+++ b/PM/Deliverables Tracking.xlsx
@@ -4,12 +4,12 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="27430"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19180" windowHeight="11100" tabRatio="500"/>
+    <workbookView xWindow="2660" yWindow="0" windowWidth="22820" windowHeight="16800" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140001" calcOnSave="0" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="46">
   <si>
     <t>The Engineer Accelerator September 2016</t>
   </si>
@@ -133,6 +133,30 @@
   </si>
   <si>
     <t>Matched Guidelines. DRC is cleared</t>
+  </si>
+  <si>
+    <t>Kiki</t>
+  </si>
+  <si>
+    <t>Yes</t>
+  </si>
+  <si>
+    <t>NA</t>
+  </si>
+  <si>
+    <t>No</t>
+  </si>
+  <si>
+    <t>Fab</t>
+  </si>
+  <si>
+    <t>Douglas</t>
+  </si>
+  <si>
+    <t>Presentation</t>
+  </si>
+  <si>
+    <t>Monique</t>
   </si>
 </sst>
 </file>
@@ -216,7 +240,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="105">
+  <cellStyleXfs count="109">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -322,8 +346,12 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -356,8 +384,11 @@
     <xf numFmtId="14" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="105">
+  <cellStyles count="109">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -410,6 +441,8 @@
     <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -462,6 +495,8 @@
     <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -859,10 +894,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D31"/>
+  <dimension ref="A1:G34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -873,22 +908,22 @@
     <col min="4" max="4" width="42.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="16">
+    <row r="1" spans="1:7" ht="16">
       <c r="A1" s="4" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="16">
+    <row r="2" spans="1:7" ht="16">
       <c r="A2" s="4" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:7">
       <c r="A4" s="6" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="5" spans="1:4">
+    <row r="5" spans="1:7">
       <c r="A5" s="7">
         <v>42630</v>
       </c>
@@ -901,8 +936,17 @@
       <c r="D5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" ht="30">
+      <c r="E5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F5" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="30">
       <c r="A6" s="8" t="s">
         <v>10</v>
       </c>
@@ -911,7 +955,7 @@
       </c>
       <c r="C6" s="6"/>
     </row>
-    <row r="7" spans="1:4">
+    <row r="7" spans="1:7">
       <c r="A7" s="5" t="s">
         <v>5</v>
       </c>
@@ -921,8 +965,14 @@
       <c r="C7" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8" s="5" t="s">
         <v>6</v>
       </c>
@@ -932,13 +982,16 @@
       <c r="C8" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="E8" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10" s="9">
         <v>42637</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30">
+    <row r="11" spans="1:7" ht="30">
       <c r="A11" s="11" t="s">
         <v>12</v>
       </c>
@@ -949,7 +1002,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="1:4">
+    <row r="12" spans="1:7">
       <c r="A12" s="11" t="s">
         <v>13</v>
       </c>
@@ -960,7 +1013,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="13" spans="1:4">
+    <row r="13" spans="1:7">
       <c r="A13" s="11" t="s">
         <v>11</v>
       </c>
@@ -971,7 +1024,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="60">
+    <row r="14" spans="1:7" ht="60">
       <c r="A14" s="5" t="s">
         <v>9</v>
       </c>
@@ -984,8 +1037,14 @@
       <c r="D14" s="5" t="s">
         <v>31</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" ht="30">
+      <c r="E14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" ht="30">
       <c r="A15" s="11" t="s">
         <v>24</v>
       </c>
@@ -996,7 +1055,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:4">
+    <row r="16" spans="1:7">
       <c r="A16" s="5" t="s">
         <v>7</v>
       </c>
@@ -1006,8 +1065,17 @@
       <c r="C16" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="17" spans="1:4">
+      <c r="E16" t="s">
+        <v>39</v>
+      </c>
+      <c r="F16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G16" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7">
       <c r="A17" s="5" t="s">
         <v>8</v>
       </c>
@@ -1017,8 +1085,14 @@
       <c r="C17" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="18" spans="1:4">
+      <c r="E17" t="s">
+        <v>39</v>
+      </c>
+      <c r="F17" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7">
       <c r="A18" s="5" t="s">
         <v>17</v>
       </c>
@@ -1031,8 +1105,14 @@
       <c r="D18" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="19" spans="1:4">
+      <c r="E18" t="s">
+        <v>39</v>
+      </c>
+      <c r="F18" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7">
       <c r="A19" s="5" t="s">
         <v>14</v>
       </c>
@@ -1045,8 +1125,17 @@
       <c r="D19" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="20" spans="1:4">
+      <c r="E19" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7">
       <c r="A20" s="3" t="s">
         <v>15</v>
       </c>
@@ -1059,8 +1148,14 @@
       <c r="D20" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="21" spans="1:4">
+      <c r="E20" t="s">
+        <v>39</v>
+      </c>
+      <c r="F20" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="21" spans="1:7">
       <c r="A21" s="3" t="s">
         <v>16</v>
       </c>
@@ -1070,8 +1165,11 @@
       <c r="C21" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="22" spans="1:4">
+      <c r="E21" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="22" spans="1:7">
       <c r="A22" s="3" t="s">
         <v>18</v>
       </c>
@@ -1081,8 +1179,11 @@
       <c r="C22" s="5" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:4">
+      <c r="E22" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="23" spans="1:7">
       <c r="A23" s="3" t="s">
         <v>34</v>
       </c>
@@ -1093,12 +1194,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="25" spans="1:4">
+    <row r="25" spans="1:7">
       <c r="A25" s="13">
         <v>42644</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30">
+    <row r="26" spans="1:7" ht="30">
       <c r="A26" s="11" t="s">
         <v>25</v>
       </c>
@@ -1109,7 +1210,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="30">
+    <row r="27" spans="1:7" ht="30">
       <c r="A27" s="11" t="s">
         <v>28</v>
       </c>
@@ -1120,7 +1221,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="28" spans="1:4">
+    <row r="28" spans="1:7">
       <c r="A28" s="5" t="s">
         <v>27</v>
       </c>
@@ -1131,7 +1232,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="29" spans="1:4">
+    <row r="29" spans="1:7">
       <c r="A29" s="5" t="s">
         <v>22</v>
       </c>
@@ -1141,8 +1242,11 @@
       <c r="C29" s="5" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="30" spans="1:4">
+      <c r="E29" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7">
       <c r="A30" s="5" t="s">
         <v>23</v>
       </c>
@@ -1153,7 +1257,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="31" spans="1:4">
+    <row r="31" spans="1:7">
       <c r="A31" s="5" t="s">
         <v>26</v>
       </c>
@@ -1161,6 +1265,22 @@
         <v>42650</v>
       </c>
       <c r="C31" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33" s="14">
+        <v>42651</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="B34" s="12">
+        <v>42657</v>
+      </c>
+      <c r="C34" s="5" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>